<commit_message>
actualizacion planilla de calculo
</commit_message>
<xml_diff>
--- a/app/datos_pwm.xlsx
+++ b/app/datos_pwm.xlsx
@@ -16,10 +16,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>X</t>
+    <t>PWM</t>
   </si>
   <si>
-    <t>Y</t>
+    <t>ADC</t>
   </si>
 </sst>
 </file>
@@ -86,12 +86,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -154,7 +155,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>X</c:v>
+                  <c:v>PWM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -627,11 +628,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="223213056"/>
-        <c:axId val="151952704"/>
+        <c:axId val="179637248"/>
+        <c:axId val="167600704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="223213056"/>
+        <c:axId val="179637248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -640,7 +641,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151952704"/>
+        <c:crossAx val="167600704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -648,7 +649,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151952704"/>
+        <c:axId val="167600704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -659,7 +660,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="223213056"/>
+        <c:crossAx val="179637248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1192,11 +1193,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="223213568"/>
-        <c:axId val="151481152"/>
+        <c:axId val="199249920"/>
+        <c:axId val="167602432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="223213568"/>
+        <c:axId val="199249920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1205,7 +1206,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151481152"/>
+        <c:crossAx val="167602432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1213,7 +1214,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151481152"/>
+        <c:axId val="167602432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1224,7 +1225,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="223213568"/>
+        <c:crossAx val="199249920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1648,10 +1649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M149"/>
+  <dimension ref="A1:Q149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1784,7 +1785,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>32768</v>
       </c>
@@ -1792,7 +1793,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>34816</v>
       </c>
@@ -1800,7 +1801,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>36864</v>
       </c>
@@ -1808,7 +1809,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>38912</v>
       </c>
@@ -1816,23 +1817,25 @@
         <v>716</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>40960</v>
       </c>
       <c r="B21">
         <v>729</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q21" s="3"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>43008</v>
       </c>
       <c r="B22">
         <v>734</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>45056</v>
       </c>
@@ -1841,7 +1844,7 @@
       </c>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>47104</v>
       </c>
@@ -1849,7 +1852,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>49152</v>
       </c>
@@ -1857,7 +1860,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>51200</v>
       </c>
@@ -1865,7 +1868,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>53248</v>
       </c>
@@ -1873,7 +1876,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>55296</v>
       </c>
@@ -1881,7 +1884,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>57344</v>
       </c>
@@ -1889,7 +1892,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>59392</v>
       </c>
@@ -1897,7 +1900,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>61440</v>
       </c>
@@ -1905,7 +1908,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>63488</v>
       </c>

</xml_diff>